<commit_message>
user: TOMS v1 DONE
</commit_message>
<xml_diff>
--- a/public/Template Pegawai Import.xlsx
+++ b/public/Template Pegawai Import.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fisip/Documents/Mervin/Traktor Nusantara/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F69455D4-DAA4-4A4F-88BF-7CEBA8D422CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15186351-F7CB-F048-8781-5F7D379E3F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16940" xr2:uid="{743E4E1D-8380-9C48-9BE3-42A78839F1B3}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="17500" xr2:uid="{B01E1EB5-CB78-9C44-B3D0-42478B67369B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" iterate="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$X$1</definedName>
+  </definedNames>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -80,15 +83,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Tanggal Lahir</t>
-  </si>
-  <si>
-    <t>Tanggal Masuk TN/SHN</t>
-  </si>
-  <si>
-    <t>Tanggal Masuk Vendor</t>
-  </si>
-  <si>
     <t>Jenis Kontrak Kerjasama</t>
   </si>
   <si>
@@ -108,6 +102,15 @@
   </si>
   <si>
     <t>No hp</t>
+  </si>
+  <si>
+    <t>Tanggal Masuk TN/SHN  (YYYY-MM-DD)</t>
+  </si>
+  <si>
+    <t>Tanggal Masuk Vendor (YYYY-MM-DD)</t>
+  </si>
+  <si>
+    <t>Tanggal Lahir (YYYY-MM-DD)</t>
   </si>
 </sst>
 </file>
@@ -123,15 +126,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
+      <sz val="13"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -156,17 +157,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 4" xfId="1" xr:uid="{10E704B8-CD33-FE49-9608-2902368A9D27}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -497,16 +499,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2A9F28-3270-A144-BCBC-0F9ED72E24F9}">
-  <dimension ref="A1:Y2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4983A550-22F4-B54A-A185-6F62DEF4E7DA}">
+  <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,63 +577,35 @@
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>